<commit_message>
Reset global correlating, more data
</commit_message>
<xml_diff>
--- a/Prediction Accuracy Data.xlsx
+++ b/Prediction Accuracy Data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">Case</t>
   </si>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">compitomin</t>
   </si>
   <si>
-    <t xml:space="preserve">Copyvet1_10</t>
+    <t xml:space="preserve">copyvet1_10</t>
   </si>
   <si>
     <t xml:space="preserve">copyvet50disp</t>
@@ -61,6 +61,9 @@
     <t xml:space="preserve">vet20parinum</t>
   </si>
   <si>
+    <t xml:space="preserve">matrixmult</t>
+  </si>
+  <si>
     <t xml:space="preserve">(0, 1)</t>
   </si>
   <si>
@@ -68,6 +71,42 @@
   </si>
   <si>
     <t xml:space="preserve">(0, 3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1, 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1, 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1, 3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2, 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2, 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2, 3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(3, 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(3, 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4, 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(5, 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(8, 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(12, 2)</t>
   </si>
 </sst>
 </file>
@@ -82,6 +121,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -163,10 +203,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -178,11 +218,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="21.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="20.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="20.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.41"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.52"/>
   </cols>
@@ -227,10 +267,13 @@
       <c r="M1" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>79.411766</v>
@@ -271,7 +314,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>73.529</v>
@@ -309,10 +352,13 @@
       <c r="M3" s="0" t="n">
         <v>85.82089</v>
       </c>
+      <c r="N3" s="0" t="n">
+        <v>67.87331</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>67.64706</v>
@@ -349,6 +395,375 @@
       </c>
       <c r="M4" s="0" t="n">
         <v>85.82089</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>82.35294</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>80.952385</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>66.666667</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>86.84211</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>83.435585</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>67.567566</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>84.210526</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>73.91304</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>68.965515</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>60.714287</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>80.597015</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>73.52941</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>73.809525</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>76.666664</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>86.84211</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>87.730064</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>62.162163</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>71.42857</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>82.45614</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>65.21739</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>62.068962</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>67.85714</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>83.58209</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>67.87331</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>67.64706</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>71.42857</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>76.666664</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>86.84211</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>87.11656</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>67.567566</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>67.85714</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>80.70176</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>65.21739</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>65.51724</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>60.714287</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>82.83582</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>76.47059</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>80.952385</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>63.333332</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>86.84211</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>83.435585</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>67.567566</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>71.42857</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>82.45614</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>73.91304</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>58.62069</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>71.42857</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>83.58209</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>67.64706</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>78.57143</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>73.333336</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>85.52631</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>89.57055</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>59.45946</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>71.42857</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>80.70176</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>73.91304</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>58.62069</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>67.85714</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>82.83582</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>67.87331</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>67.64706</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>76.190475</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>73.333336</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>85.52631</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>89.57055</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>67.567566</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>60.714287</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>80.70176</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>73.91304</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>44.82787</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>60.714287</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>84.32836</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>70.588234</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>76.190475</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>88.15789</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>84.04908</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>67.567566</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>67.85714</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>64.75973</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>86.95652</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>58.62069</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>60.714287</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>82.08955</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>70.588234</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>76.190475</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>76.666664</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>86.84211</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>88.957054</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>64.86486</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>67.85714</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>72.831055</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>82.608698</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>75.86207</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>64.28571</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>84.32836</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>67.87331</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>71.49322</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <v>89.140274</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <v>93.21267</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <v>95.928605</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More data collection, display number of branches
</commit_message>
<xml_diff>
--- a/Prediction Accuracy Data.xlsx
+++ b/Prediction Accuracy Data.xlsx
@@ -205,8 +205,8 @@
   </sheetPr>
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -216,7 +216,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.13"/>
@@ -738,6 +738,9 @@
       <c r="A13" s="0" t="s">
         <v>25</v>
       </c>
+      <c r="F13" s="0" t="n">
+        <v>89.57055</v>
+      </c>
       <c r="N13" s="0" t="n">
         <v>71.49322</v>
       </c>
@@ -746,6 +749,9 @@
       <c r="A14" s="0" t="s">
         <v>26</v>
       </c>
+      <c r="F14" s="0" t="n">
+        <v>90.18405</v>
+      </c>
       <c r="N14" s="0" t="n">
         <v>89.140274</v>
       </c>
@@ -754,6 +760,9 @@
       <c r="A15" s="0" t="s">
         <v>27</v>
       </c>
+      <c r="F15" s="0" t="n">
+        <v>87.730064</v>
+      </c>
       <c r="N15" s="0" t="n">
         <v>93.21267</v>
       </c>
@@ -761,6 +770,9 @@
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>28</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>88.34356</v>
       </c>
       <c r="N16" s="0" t="n">
         <v>95.928605</v>

</xml_diff>